<commit_message>
added more data and uploading functions
</commit_message>
<xml_diff>
--- a/AURIN_data/Schema.xlsx
+++ b/AURIN_data/Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Si\Google Drive\Master of IT\Unimelb S3\Cluster and Cloud Computing\Assignment2\CloudComputing-RealEstateMarketAnalysis\AURIN_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B11B208-DCCD-469A-AB65-2E05ACBD6E1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574A943C-2388-4065-9E87-8902B3A85EFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Timeseries Property Data" sheetId="6" r:id="rId1"/>
@@ -2847,7 +2847,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2857,6 +2857,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2895,7 +2901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2908,6 +2914,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3192,7 +3201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767487B0-5AF0-47B2-B429-83C3B8C8F6DB}">
   <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
@@ -21812,13 +21821,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39574F08-F52F-4556-A387-6BEB11B523E7}">
   <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="59.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="74.88671875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
@@ -23153,14 +23162,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C37753F-F997-4D91-AFA4-DAFE2A9A2783}">
   <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="78.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="93.21875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
@@ -24489,7 +24498,7 @@
       <c r="A122" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="6" t="s">
         <v>409</v>
       </c>
       <c r="C122" s="2" t="s">
@@ -24555,7 +24564,7 @@
       <c r="A128" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" s="6" t="s">
         <v>421</v>
       </c>
       <c r="C128" s="2" t="s">
@@ -24742,7 +24751,7 @@
       <c r="A145" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B145" s="6" t="s">
         <v>455</v>
       </c>
       <c r="C145" s="2" t="s">

</xml_diff>